<commit_message>
Working on salto show
</commit_message>
<xml_diff>
--- a/choreography/routines/template.xlsx
+++ b/choreography/routines/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="routine" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="movelist" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="routine" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="movelist" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001"/>
@@ -1472,7 +1472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:B137"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="B15" s="23" t="inlineStr">
         <is>
-          <t>340533</t>
+          <t>340867</t>
         </is>
       </c>
     </row>
@@ -1717,442 +1717,1402 @@
     <row r="21" ht="12.75" customHeight="1" s="19">
       <c r="A21" s="23" t="inlineStr">
         <is>
-          <t>crawl_scorpion.csv</t>
+          <t>act_moveyourfeet_v4.csv</t>
         </is>
       </c>
       <c r="B21" s="23" t="inlineStr">
         <is>
-          <t>1767</t>
+          <t>114500</t>
         </is>
       </c>
     </row>
     <row r="22" ht="12.75" customHeight="1" s="19">
       <c r="A22" s="23" t="inlineStr">
         <is>
-          <t>crawl_sit.csv</t>
+          <t>act_salto_p2_dans_acro_02.csv</t>
         </is>
       </c>
       <c r="B22" s="23" t="inlineStr">
         <is>
-          <t>833</t>
+          <t>127033</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>dance_aloof.csv</t>
+          <t>act_salto_p4_flipover.csv</t>
         </is>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>17667</t>
+          <t>13800</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>greeting_bow_deep.csv</t>
+          <t>act_salto_p4_hit.csv</t>
         </is>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>6400</t>
+          <t>500</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>greeting_bow_small.csv</t>
+          <t>act_salto_p4_kick.csv</t>
         </is>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>2833</t>
+          <t>700</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>greeting_nod.csv</t>
+          <t>Ars hump front low.csv</t>
         </is>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>933</t>
+          <t>6900</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>greeting_shake_hand.csv</t>
+          <t>ars_back_stretch.csv</t>
         </is>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>6900</t>
+          <t>114867</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>greeting_wave_double.csv</t>
+          <t>ars_headstand.csv</t>
         </is>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>6133</t>
+          <t>79367</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>greeting_wave_left.csv</t>
+          <t>Ars_hump_front_low.csv</t>
         </is>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>6133</t>
+          <t>16200</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>pose_180.csv</t>
+          <t>ars_repeat_rotate_arms_legs_samedir_16s.csv</t>
         </is>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>16000</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
+          <t>ars_roll_f2b.csv</t>
+        </is>
+      </c>
+      <c r="B31" s="0" t="inlineStr">
+        <is>
+          <t>5467</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="inlineStr">
+        <is>
+          <t>ars_roll_sideways_high.csv</t>
+        </is>
+      </c>
+      <c r="B32" s="0" t="inlineStr">
+        <is>
+          <t>3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="inlineStr">
+        <is>
+          <t>ars_roll_sideways_lower.csv</t>
+        </is>
+      </c>
+      <c r="B33" s="0" t="inlineStr">
+        <is>
+          <t>3933</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="inlineStr">
+        <is>
+          <t>ars_sequence_1.csv</t>
+        </is>
+      </c>
+      <c r="B34" s="0" t="inlineStr">
+        <is>
+          <t>648000</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="inlineStr">
+        <is>
+          <t>ars_sequence_2.csv</t>
+        </is>
+      </c>
+      <c r="B35" s="0" t="inlineStr">
+        <is>
+          <t>574333</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="0" t="inlineStr">
+        <is>
+          <t>ars_situp.csv</t>
+        </is>
+      </c>
+      <c r="B36" s="0" t="inlineStr">
+        <is>
+          <t>29800</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="0" t="inlineStr">
+        <is>
+          <t>chair-handstand-dst-isolated-soft.csv</t>
+        </is>
+      </c>
+      <c r="B37" s="0" t="inlineStr">
+        <is>
+          <t>17267</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="0" t="inlineStr">
+        <is>
+          <t>chair-handstand-dst-isolated.csv</t>
+        </is>
+      </c>
+      <c r="B38" s="0" t="inlineStr">
+        <is>
+          <t>17267</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="0" t="inlineStr">
+        <is>
+          <t>chair-to-handstand.csv</t>
+        </is>
+      </c>
+      <c r="B39" s="0" t="inlineStr">
+        <is>
+          <t>21967</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="0" t="inlineStr">
+        <is>
+          <t>circusstad_acro.csv</t>
+        </is>
+      </c>
+      <c r="B40" s="0" t="inlineStr">
+        <is>
+          <t>367067</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="0" t="inlineStr">
+        <is>
+          <t>circusstad_acroyoga.csv</t>
+        </is>
+      </c>
+      <c r="B41" s="0" t="inlineStr">
+        <is>
+          <t>265933</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="0" t="inlineStr">
+        <is>
+          <t>circusstad_ending_alive.csv</t>
+        </is>
+      </c>
+      <c r="B42" s="0" t="inlineStr">
+        <is>
+          <t>145467</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="0" t="inlineStr">
+        <is>
+          <t>circusstad_microphone.csv</t>
+        </is>
+      </c>
+      <c r="B43" s="0" t="inlineStr">
+        <is>
+          <t>70267</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="0" t="inlineStr">
+        <is>
+          <t>circusstad_spiegelen.csv</t>
+        </is>
+      </c>
+      <c r="B44" s="0" t="inlineStr">
+        <is>
+          <t>199667</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="0" t="inlineStr">
+        <is>
+          <t>circusstad_spiegel_acroyoga.csv</t>
+        </is>
+      </c>
+      <c r="B45" s="0" t="inlineStr">
+        <is>
+          <t>465400</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="0" t="inlineStr">
+        <is>
+          <t>circusstad_spiegel_acroyoga_adjusted.csv</t>
+        </is>
+      </c>
+      <c r="B46" s="0" t="inlineStr">
+        <is>
+          <t>413033</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="0" t="inlineStr">
+        <is>
+          <t>circusstad_spiegel_acroyoga_shorter.csv</t>
+        </is>
+      </c>
+      <c r="B47" s="0" t="inlineStr">
+        <is>
+          <t>401367</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="0" t="inlineStr">
+        <is>
+          <t>circusstad_spiegel_acroyoga_shorter_long_in.csv</t>
+        </is>
+      </c>
+      <c r="B48" s="0" t="inlineStr">
+        <is>
+          <t>465467</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="0" t="inlineStr">
+        <is>
+          <t>crawl_scorpion.csv</t>
+        </is>
+      </c>
+      <c r="B49" s="0" t="inlineStr">
+        <is>
+          <t>1767</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="0" t="inlineStr">
+        <is>
+          <t>crawl_sit.csv</t>
+        </is>
+      </c>
+      <c r="B50" s="0" t="inlineStr">
+        <is>
+          <t>833</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="0" t="inlineStr">
+        <is>
+          <t>dance_aloof.csv</t>
+        </is>
+      </c>
+      <c r="B51" s="0" t="inlineStr">
+        <is>
+          <t>17667</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0" t="inlineStr">
+        <is>
+          <t>dst-after-handstand-isolated.csv</t>
+        </is>
+      </c>
+      <c r="B52" s="0" t="inlineStr">
+        <is>
+          <t>65700</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0" t="inlineStr">
+        <is>
+          <t>dst-backturn-to-standing-isolated.csv</t>
+        </is>
+      </c>
+      <c r="B53" s="0" t="inlineStr">
+        <is>
+          <t>7333</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0" t="inlineStr">
+        <is>
+          <t>dst-craddle-walkover.csv</t>
+        </is>
+      </c>
+      <c r="B54" s="0" t="inlineStr">
+        <is>
+          <t>9067</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0" t="inlineStr">
+        <is>
+          <t>dst-foot-play.csv</t>
+        </is>
+      </c>
+      <c r="B55" s="0" t="inlineStr">
+        <is>
+          <t>56067</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0" t="inlineStr">
+        <is>
+          <t>FGT_lets_dance.csv</t>
+        </is>
+      </c>
+      <c r="B56" s="0" t="inlineStr">
+        <is>
+          <t>142333</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="0" t="inlineStr">
+        <is>
+          <t>greetings_wave.csv</t>
+        </is>
+      </c>
+      <c r="B57" s="0" t="inlineStr">
+        <is>
+          <t>7500</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0" t="inlineStr">
+        <is>
+          <t>greeting_bow_deep.csv</t>
+        </is>
+      </c>
+      <c r="B58" s="0" t="inlineStr">
+        <is>
+          <t>6400</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0" t="inlineStr">
+        <is>
+          <t>greeting_bow_small.csv</t>
+        </is>
+      </c>
+      <c r="B59" s="0" t="inlineStr">
+        <is>
+          <t>2833</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0" t="inlineStr">
+        <is>
+          <t>greeting_nod.csv</t>
+        </is>
+      </c>
+      <c r="B60" s="0" t="inlineStr">
+        <is>
+          <t>933</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0" t="inlineStr">
+        <is>
+          <t>greeting_shake_hand.csv</t>
+        </is>
+      </c>
+      <c r="B61" s="0" t="inlineStr">
+        <is>
+          <t>6900</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="0" t="inlineStr">
+        <is>
+          <t>greeting_wave_double.csv</t>
+        </is>
+      </c>
+      <c r="B62" s="0" t="inlineStr">
+        <is>
+          <t>6133</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="0" t="inlineStr">
+        <is>
+          <t>greeting_wave_left.csv</t>
+        </is>
+      </c>
+      <c r="B63" s="0" t="inlineStr">
+        <is>
+          <t>6133</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="0" t="inlineStr">
+        <is>
+          <t>iso-f2h-catch-rockroll-seq.csv</t>
+        </is>
+      </c>
+      <c r="B64" s="0" t="inlineStr">
+        <is>
+          <t>29967</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="0" t="inlineStr">
+        <is>
+          <t>iso-forhead-balance.csv</t>
+        </is>
+      </c>
+      <c r="B65" s="0" t="inlineStr">
+        <is>
+          <t>8400</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="0" t="inlineStr">
+        <is>
+          <t>iso-lowh2h-standonshoulder.csv</t>
+        </is>
+      </c>
+      <c r="B66" s="0" t="inlineStr">
+        <is>
+          <t>43100</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="0" t="inlineStr">
+        <is>
+          <t>iso-shoulderbird-kneehandstand.csv</t>
+        </is>
+      </c>
+      <c r="B67" s="0" t="inlineStr">
+        <is>
+          <t>22167</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="0" t="inlineStr">
+        <is>
+          <t>pattern-3-limbs-referentie.csv</t>
+        </is>
+      </c>
+      <c r="B68" s="0" t="inlineStr">
+        <is>
+          <t>3333</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="0" t="inlineStr">
+        <is>
+          <t>pattern-3-limbs.csv</t>
+        </is>
+      </c>
+      <c r="B69" s="0" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="0" t="inlineStr">
+        <is>
+          <t>pattern-3-limbs2.csv</t>
+        </is>
+      </c>
+      <c r="B70" s="0" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="0" t="inlineStr">
+        <is>
+          <t>pose_180.csv</t>
+        </is>
+      </c>
+      <c r="B71" s="0" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="0" t="inlineStr">
+        <is>
           <t>pose_handstand.csv</t>
         </is>
       </c>
-      <c r="B31" s="0" t="inlineStr">
+      <c r="B72" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
+    <row r="73">
+      <c r="A73" s="0" t="inlineStr">
         <is>
           <t>pose_handstand_oversplit.csv</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="B73" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
+    <row r="74">
+      <c r="A74" s="0" t="inlineStr">
         <is>
           <t>pose_handstand_split.csv</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B74" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
+    <row r="75">
+      <c r="A75" s="0" t="inlineStr">
         <is>
           <t>pose_planche.csv</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B75" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+    <row r="76">
+      <c r="A76" s="0" t="inlineStr">
         <is>
           <t>pose_scorpion.csv</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="B76" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
+    <row r="77">
+      <c r="A77" s="0" t="inlineStr">
         <is>
           <t>pose_seven.csv</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="B77" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
+    <row r="78">
+      <c r="A78" s="0" t="inlineStr">
         <is>
           <t>pose_sit.csv</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B78" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+    <row r="79">
+      <c r="A79" s="0" t="inlineStr">
         <is>
           <t>pose_split_l.csv</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B79" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
+    <row r="80">
+      <c r="A80" s="0" t="inlineStr">
         <is>
           <t>pose_stand.csv</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B80" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
+    <row r="81">
+      <c r="A81" s="0" t="inlineStr">
         <is>
           <t>pose_stand_legs_only.csv</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="B81" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
+    <row r="82">
+      <c r="A82" s="0" t="inlineStr">
         <is>
           <t>pose_table.csv</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B82" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
+    <row r="83">
+      <c r="A83" s="0" t="inlineStr">
         <is>
           <t>pose_yoga_dog.csv</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="B83" s="0" t="inlineStr">
         <is>
           <t>33</t>
         </is>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
+    <row r="84">
+      <c r="A84" s="0" t="inlineStr">
+        <is>
+          <t>quick_01-backup.csv</t>
+        </is>
+      </c>
+      <c r="B84" s="0" t="inlineStr">
+        <is>
+          <t>102833</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="0" t="inlineStr">
+        <is>
+          <t>repeat_hump_arms_legs_samedir_16s.csv</t>
+        </is>
+      </c>
+      <c r="B85" s="0" t="inlineStr">
+        <is>
+          <t>16000</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="0" t="inlineStr">
+        <is>
+          <t>repeat_hump_large_4s.csv</t>
+        </is>
+      </c>
+      <c r="B86" s="0" t="inlineStr">
+        <is>
+          <t>4000</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="0" t="inlineStr">
+        <is>
+          <t>repeat_hump_medium_3s.csv</t>
+        </is>
+      </c>
+      <c r="B87" s="0" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="0" t="inlineStr">
+        <is>
+          <t>repeat_hump_medium_arms_3s.csv</t>
+        </is>
+      </c>
+      <c r="B88" s="0" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="0" t="inlineStr">
+        <is>
+          <t>repeat_hump_medium_arms_linear_3s.csv</t>
+        </is>
+      </c>
+      <c r="B89" s="0" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="0" t="inlineStr">
+        <is>
+          <t>repeat_hump_medium_windup_5s.csv</t>
+        </is>
+      </c>
+      <c r="B90" s="0" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="0" t="inlineStr">
+        <is>
+          <t>repeat_hump_small_1s.csv</t>
+        </is>
+      </c>
+      <c r="B91" s="0" t="inlineStr">
+        <is>
+          <t>1000</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="0" t="inlineStr">
+        <is>
+          <t>repeat_hump_small_3s.csv</t>
+        </is>
+      </c>
+      <c r="B92" s="0" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="0" t="inlineStr">
+        <is>
+          <t>repeat_hump_XL_4s.csv</t>
+        </is>
+      </c>
+      <c r="B93" s="0" t="inlineStr">
+        <is>
+          <t>4000</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="0" t="inlineStr">
+        <is>
+          <t>repeat_random_individual_10s.csv</t>
+        </is>
+      </c>
+      <c r="B94" s="0" t="inlineStr">
+        <is>
+          <t>10000</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="0" t="inlineStr">
+        <is>
+          <t>repeat_random_individual_20s.csv</t>
+        </is>
+      </c>
+      <c r="B95" s="0" t="inlineStr">
+        <is>
+          <t>20000</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="0" t="inlineStr">
+        <is>
+          <t>repeat_random_individual_ease_20s.csv</t>
+        </is>
+      </c>
+      <c r="B96" s="0" t="inlineStr">
+        <is>
+          <t>20000</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="0" t="inlineStr">
+        <is>
+          <t>repeat_random_individual_lin_20.csv</t>
+        </is>
+      </c>
+      <c r="B97" s="0" t="inlineStr">
+        <is>
+          <t>20000</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0" t="inlineStr">
+        <is>
+          <t>repeat_rotate_arms_16s.csv</t>
+        </is>
+      </c>
+      <c r="B98" s="0" t="inlineStr">
+        <is>
+          <t>16000</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0" t="inlineStr">
+        <is>
+          <t>repeat_rotate_arms_legs_opp_16s.csv</t>
+        </is>
+      </c>
+      <c r="B99" s="0" t="inlineStr">
+        <is>
+          <t>16000</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0" t="inlineStr">
+        <is>
+          <t>repeat_rotate_arms_legs_samedir_16s.csv</t>
+        </is>
+      </c>
+      <c r="B100" s="0" t="inlineStr">
+        <is>
+          <t>16000</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0" t="inlineStr">
+        <is>
+          <t>salto_d2_dans_acro_01.csv</t>
+        </is>
+      </c>
+      <c r="B101" s="0" t="inlineStr">
+        <is>
+          <t>60133</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="0" t="inlineStr">
+        <is>
+          <t>salto_d2_dans_acro_02.csv</t>
+        </is>
+      </c>
+      <c r="B102" s="0" t="inlineStr">
+        <is>
+          <t>127033</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="0" t="inlineStr">
+        <is>
+          <t>shoulderbird-knee-tweakers.csv</t>
+        </is>
+      </c>
+      <c r="B103" s="0" t="inlineStr">
+        <is>
+          <t>27967</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="0" t="inlineStr">
+        <is>
+          <t>tango-downward-dog-sequence.csv</t>
+        </is>
+      </c>
+      <c r="B104" s="0" t="inlineStr">
+        <is>
+          <t>32000</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="0" t="inlineStr">
+        <is>
+          <t>tango-sequence-dst-alternate-end.csv</t>
+        </is>
+      </c>
+      <c r="B105" s="0" t="inlineStr">
+        <is>
+          <t>110900</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="0" t="inlineStr">
+        <is>
+          <t>tango-sequence-dst-splits.csv</t>
+        </is>
+      </c>
+      <c r="B106" s="0" t="inlineStr">
+        <is>
+          <t>6500</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="0" t="inlineStr">
+        <is>
+          <t>tango-sequence-dst-splits2.csv</t>
+        </is>
+      </c>
+      <c r="B107" s="0" t="inlineStr">
+        <is>
+          <t>13500</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="0" t="inlineStr">
+        <is>
+          <t>tango-sequence-dst-stoeltje.csv</t>
+        </is>
+      </c>
+      <c r="B108" s="0" t="inlineStr">
+        <is>
+          <t>8567</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="0" t="inlineStr">
+        <is>
+          <t>tango-sequence-dst.csv</t>
+        </is>
+      </c>
+      <c r="B109" s="0" t="inlineStr">
+        <is>
+          <t>112233</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="0" t="inlineStr">
+        <is>
+          <t>test_3limbs.csv</t>
+        </is>
+      </c>
+      <c r="B110" s="0" t="inlineStr">
+        <is>
+          <t>4000</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="0" t="inlineStr">
         <is>
           <t>test_cannonball.csv</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B111" s="0" t="inlineStr">
         <is>
           <t>24367</t>
         </is>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
+    <row r="112">
+      <c r="A112" s="0" t="inlineStr">
         <is>
           <t>test_contra_finale.csv</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B112" s="0" t="inlineStr">
         <is>
           <t>40833</t>
         </is>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
+    <row r="113">
+      <c r="A113" s="0" t="inlineStr">
+        <is>
+          <t>test_dog.csv</t>
+        </is>
+      </c>
+      <c r="B113" s="0" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="0" t="inlineStr">
         <is>
           <t>test_flikflak_daniel.csv</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
+      <c r="B114" s="0" t="inlineStr">
         <is>
           <t>22633</t>
         </is>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
+    <row r="115">
+      <c r="A115" s="0" t="inlineStr">
         <is>
           <t>test_flop_roll.csv</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
+      <c r="B115" s="0" t="inlineStr">
         <is>
           <t>10100</t>
         </is>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
+    <row r="116">
+      <c r="A116" s="0" t="inlineStr">
+        <is>
+          <t>test_fullrev.csv</t>
+        </is>
+      </c>
+      <c r="B116" s="0" t="inlineStr">
+        <is>
+          <t>8000</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="0" t="inlineStr">
+        <is>
+          <t>test_multi_rev.csv</t>
+        </is>
+      </c>
+      <c r="B117" s="0" t="inlineStr">
+        <is>
+          <t>20000</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="0" t="inlineStr">
         <is>
           <t>test_rockroll.csv</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
+      <c r="B118" s="0" t="inlineStr">
         <is>
           <t>32967</t>
         </is>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
+    <row r="119">
+      <c r="A119" s="0" t="inlineStr">
         <is>
           <t>travel_walk_96bmp.csv</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B119" s="0" t="inlineStr">
         <is>
           <t>1333</t>
         </is>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
+    <row r="120">
+      <c r="A120" s="0" t="inlineStr">
+        <is>
+          <t>trick-backflip-pose.csv</t>
+        </is>
+      </c>
+      <c r="B120" s="0" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="0" t="inlineStr">
+        <is>
+          <t>trick-backflip1.csv</t>
+        </is>
+      </c>
+      <c r="B121" s="0" t="inlineStr">
+        <is>
+          <t>7933</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="0" t="inlineStr">
+        <is>
+          <t>trick-backflip2.csv</t>
+        </is>
+      </c>
+      <c r="B122" s="0" t="inlineStr">
+        <is>
+          <t>12033</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="0" t="inlineStr">
+        <is>
+          <t>trick-backflip3.csv</t>
+        </is>
+      </c>
+      <c r="B123" s="0" t="inlineStr">
+        <is>
+          <t>13033</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="0" t="inlineStr">
+        <is>
+          <t>trick-backflip4.csv</t>
+        </is>
+      </c>
+      <c r="B124" s="0" t="inlineStr">
+        <is>
+          <t>13033</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="0" t="inlineStr">
+        <is>
+          <t>trick-ropeskipping.csv</t>
+        </is>
+      </c>
+      <c r="B125" s="0" t="inlineStr">
+        <is>
+          <t>7000</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="0" t="inlineStr">
+        <is>
+          <t>trick-ropeskipping2.csv</t>
+        </is>
+      </c>
+      <c r="B126" s="0" t="inlineStr">
+        <is>
+          <t>3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="0" t="inlineStr">
+        <is>
+          <t>trick-walkover.csv</t>
+        </is>
+      </c>
+      <c r="B127" s="0" t="inlineStr">
+        <is>
+          <t>21000</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="0" t="inlineStr">
+        <is>
+          <t>trick-walkover2.csv</t>
+        </is>
+      </c>
+      <c r="B128" s="0" t="inlineStr">
+        <is>
+          <t>18000</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="0" t="inlineStr">
         <is>
           <t>walk_backwards.csv</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B129" s="0" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
+    <row r="130">
+      <c r="A130" s="0" t="inlineStr">
         <is>
           <t>walk_forwards.csv</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B130" s="0" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
+    <row r="131">
+      <c r="A131" s="0" t="inlineStr">
         <is>
           <t>walk_large.csv</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
+      <c r="B131" s="0" t="inlineStr">
         <is>
           <t>2000</t>
         </is>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
+    <row r="132">
+      <c r="A132" s="0" t="inlineStr">
         <is>
           <t>walk_normal.csv</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
+      <c r="B132" s="0" t="inlineStr">
         <is>
           <t>1600</t>
         </is>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
+    <row r="133">
+      <c r="A133" s="0" t="inlineStr">
         <is>
           <t>walk_zombie.csv</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
+      <c r="B133" s="0" t="inlineStr">
         <is>
           <t>1600</t>
         </is>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
+    <row r="134">
+      <c r="A134" t="inlineStr">
         <is>
           <t>warmup_arm_swing.csv</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
+      <c r="B134" t="inlineStr">
         <is>
           <t>23867</t>
         </is>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
+    <row r="135">
+      <c r="A135" t="inlineStr">
         <is>
           <t>warmup_leg_stretch.csv</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B135" t="inlineStr">
         <is>
           <t>19467</t>
         </is>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
+    <row r="136">
+      <c r="A136" t="inlineStr">
         <is>
           <t>warmup_shoulder_stretch.csv</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
+      <c r="B136" t="inlineStr">
         <is>
           <t>15267</t>
         </is>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
+    <row r="137">
+      <c r="A137" t="inlineStr">
         <is>
           <t>warmup_situp.csv</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
+      <c r="B137" t="inlineStr">
         <is>
           <t>5900</t>
         </is>

</xml_diff>

<commit_message>
Working on salto act
</commit_message>
<xml_diff>
--- a/choreography/routines/template.xlsx
+++ b/choreography/routines/template.xlsx
@@ -1472,7 +1472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:B137"/>
+  <dimension ref="A1:B142"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
@@ -1734,650 +1734,650 @@
       </c>
       <c r="B22" s="23" t="inlineStr">
         <is>
-          <t>127033</t>
+          <t>135433</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>act_salto_p4_flipover.csv</t>
+          <t>act_salto_p2_dans_acro_03.csv</t>
         </is>
       </c>
       <c r="B23" s="0" t="inlineStr">
         <is>
-          <t>13800</t>
+          <t>135633</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>act_salto_p4_hit.csv</t>
+          <t>act_salto_p4_flipover.csv</t>
         </is>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>500</t>
+          <t>9167</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>act_salto_p4_kick.csv</t>
+          <t>act_salto_p4_hit.csv</t>
         </is>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>700</t>
+          <t>500</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>Ars hump front low.csv</t>
+          <t>act_salto_p4_hit_02.csv</t>
         </is>
       </c>
       <c r="B26" s="0" t="inlineStr">
         <is>
-          <t>6900</t>
+          <t>600</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>ars_back_stretch.csv</t>
+          <t>act_salto_p4_kick.csv</t>
         </is>
       </c>
       <c r="B27" s="0" t="inlineStr">
         <is>
-          <t>114867</t>
+          <t>700</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0" t="inlineStr">
         <is>
-          <t>ars_headstand.csv</t>
+          <t>act_salto_p5_overload.csv</t>
         </is>
       </c>
       <c r="B28" s="0" t="inlineStr">
         <is>
-          <t>79367</t>
+          <t>39967</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="0" t="inlineStr">
         <is>
-          <t>Ars_hump_front_low.csv</t>
+          <t>act_salto_p6_finale.csv</t>
         </is>
       </c>
       <c r="B29" s="0" t="inlineStr">
         <is>
-          <t>16200</t>
+          <t>103067</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="inlineStr">
         <is>
-          <t>ars_repeat_rotate_arms_legs_samedir_16s.csv</t>
+          <t>act_salto_test_shake.csv</t>
         </is>
       </c>
       <c r="B30" s="0" t="inlineStr">
         <is>
-          <t>16000</t>
+          <t>21967</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="inlineStr">
         <is>
-          <t>ars_roll_f2b.csv</t>
+          <t>Ars hump front low.csv</t>
         </is>
       </c>
       <c r="B31" s="0" t="inlineStr">
         <is>
-          <t>5467</t>
+          <t>6900</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0" t="inlineStr">
         <is>
-          <t>ars_roll_sideways_high.csv</t>
+          <t>ars_back_stretch.csv</t>
         </is>
       </c>
       <c r="B32" s="0" t="inlineStr">
         <is>
-          <t>3500</t>
+          <t>114867</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0" t="inlineStr">
         <is>
-          <t>ars_roll_sideways_lower.csv</t>
+          <t>ars_headstand.csv</t>
         </is>
       </c>
       <c r="B33" s="0" t="inlineStr">
         <is>
-          <t>3933</t>
+          <t>79367</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0" t="inlineStr">
         <is>
-          <t>ars_sequence_1.csv</t>
+          <t>Ars_hump_front_low.csv</t>
         </is>
       </c>
       <c r="B34" s="0" t="inlineStr">
         <is>
-          <t>648000</t>
+          <t>16200</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0" t="inlineStr">
         <is>
-          <t>ars_sequence_2.csv</t>
+          <t>ars_repeat_rotate_arms_legs_samedir_16s.csv</t>
         </is>
       </c>
       <c r="B35" s="0" t="inlineStr">
         <is>
-          <t>574333</t>
+          <t>16000</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0" t="inlineStr">
         <is>
-          <t>ars_situp.csv</t>
+          <t>ars_roll_f2b.csv</t>
         </is>
       </c>
       <c r="B36" s="0" t="inlineStr">
         <is>
-          <t>29800</t>
+          <t>5467</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0" t="inlineStr">
         <is>
-          <t>chair-handstand-dst-isolated-soft.csv</t>
+          <t>ars_roll_sideways_high.csv</t>
         </is>
       </c>
       <c r="B37" s="0" t="inlineStr">
         <is>
-          <t>17267</t>
+          <t>3500</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0" t="inlineStr">
         <is>
-          <t>chair-handstand-dst-isolated.csv</t>
+          <t>ars_roll_sideways_lower.csv</t>
         </is>
       </c>
       <c r="B38" s="0" t="inlineStr">
         <is>
-          <t>17267</t>
+          <t>3933</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0" t="inlineStr">
         <is>
-          <t>chair-to-handstand.csv</t>
+          <t>ars_sequence_1.csv</t>
         </is>
       </c>
       <c r="B39" s="0" t="inlineStr">
         <is>
-          <t>21967</t>
+          <t>648000</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0" t="inlineStr">
         <is>
-          <t>circusstad_acro.csv</t>
+          <t>ars_sequence_2.csv</t>
         </is>
       </c>
       <c r="B40" s="0" t="inlineStr">
         <is>
-          <t>367067</t>
+          <t>574333</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="0" t="inlineStr">
         <is>
-          <t>circusstad_acroyoga.csv</t>
+          <t>ars_situp.csv</t>
         </is>
       </c>
       <c r="B41" s="0" t="inlineStr">
         <is>
-          <t>265933</t>
+          <t>29800</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0" t="inlineStr">
         <is>
-          <t>circusstad_ending_alive.csv</t>
+          <t>chair-handstand-dst-isolated-soft.csv</t>
         </is>
       </c>
       <c r="B42" s="0" t="inlineStr">
         <is>
-          <t>145467</t>
+          <t>17267</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0" t="inlineStr">
         <is>
-          <t>circusstad_microphone.csv</t>
+          <t>chair-handstand-dst-isolated.csv</t>
         </is>
       </c>
       <c r="B43" s="0" t="inlineStr">
         <is>
-          <t>70267</t>
+          <t>17267</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0" t="inlineStr">
         <is>
-          <t>circusstad_spiegelen.csv</t>
+          <t>chair-to-handstand.csv</t>
         </is>
       </c>
       <c r="B44" s="0" t="inlineStr">
         <is>
-          <t>199667</t>
+          <t>21967</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0" t="inlineStr">
         <is>
-          <t>circusstad_spiegel_acroyoga.csv</t>
+          <t>circusstad_acro.csv</t>
         </is>
       </c>
       <c r="B45" s="0" t="inlineStr">
         <is>
-          <t>465400</t>
+          <t>367067</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0" t="inlineStr">
         <is>
-          <t>circusstad_spiegel_acroyoga_adjusted.csv</t>
+          <t>circusstad_acroyoga.csv</t>
         </is>
       </c>
       <c r="B46" s="0" t="inlineStr">
         <is>
-          <t>413033</t>
+          <t>265933</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0" t="inlineStr">
         <is>
-          <t>circusstad_spiegel_acroyoga_shorter.csv</t>
+          <t>circusstad_ending_alive.csv</t>
         </is>
       </c>
       <c r="B47" s="0" t="inlineStr">
         <is>
-          <t>401367</t>
+          <t>145467</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0" t="inlineStr">
         <is>
-          <t>circusstad_spiegel_acroyoga_shorter_long_in.csv</t>
+          <t>circusstad_microphone.csv</t>
         </is>
       </c>
       <c r="B48" s="0" t="inlineStr">
         <is>
-          <t>465467</t>
+          <t>70267</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0" t="inlineStr">
         <is>
-          <t>crawl_scorpion.csv</t>
+          <t>circusstad_spiegelen.csv</t>
         </is>
       </c>
       <c r="B49" s="0" t="inlineStr">
         <is>
-          <t>1767</t>
+          <t>199667</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="inlineStr">
         <is>
-          <t>crawl_sit.csv</t>
+          <t>circusstad_spiegel_acroyoga.csv</t>
         </is>
       </c>
       <c r="B50" s="0" t="inlineStr">
         <is>
-          <t>833</t>
+          <t>465400</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="0" t="inlineStr">
         <is>
-          <t>dance_aloof.csv</t>
+          <t>circusstad_spiegel_acroyoga_adjusted.csv</t>
         </is>
       </c>
       <c r="B51" s="0" t="inlineStr">
         <is>
-          <t>17667</t>
+          <t>413033</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="0" t="inlineStr">
         <is>
-          <t>dst-after-handstand-isolated.csv</t>
+          <t>circusstad_spiegel_acroyoga_shorter.csv</t>
         </is>
       </c>
       <c r="B52" s="0" t="inlineStr">
         <is>
-          <t>65700</t>
+          <t>401367</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="0" t="inlineStr">
         <is>
-          <t>dst-backturn-to-standing-isolated.csv</t>
+          <t>circusstad_spiegel_acroyoga_shorter_long_in.csv</t>
         </is>
       </c>
       <c r="B53" s="0" t="inlineStr">
         <is>
-          <t>7333</t>
+          <t>465467</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="0" t="inlineStr">
         <is>
-          <t>dst-craddle-walkover.csv</t>
+          <t>crawl_scorpion.csv</t>
         </is>
       </c>
       <c r="B54" s="0" t="inlineStr">
         <is>
-          <t>9067</t>
+          <t>1767</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="0" t="inlineStr">
         <is>
-          <t>dst-foot-play.csv</t>
+          <t>crawl_sit.csv</t>
         </is>
       </c>
       <c r="B55" s="0" t="inlineStr">
         <is>
-          <t>56067</t>
+          <t>833</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="0" t="inlineStr">
         <is>
-          <t>FGT_lets_dance.csv</t>
+          <t>dance_aloof.csv</t>
         </is>
       </c>
       <c r="B56" s="0" t="inlineStr">
         <is>
-          <t>142333</t>
+          <t>17667</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="0" t="inlineStr">
         <is>
-          <t>greetings_wave.csv</t>
+          <t>dst-after-handstand-isolated.csv</t>
         </is>
       </c>
       <c r="B57" s="0" t="inlineStr">
         <is>
-          <t>7500</t>
+          <t>65700</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="0" t="inlineStr">
         <is>
-          <t>greeting_bow_deep.csv</t>
+          <t>dst-backturn-to-standing-isolated.csv</t>
         </is>
       </c>
       <c r="B58" s="0" t="inlineStr">
         <is>
-          <t>6400</t>
+          <t>7333</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="0" t="inlineStr">
         <is>
-          <t>greeting_bow_small.csv</t>
+          <t>dst-craddle-walkover.csv</t>
         </is>
       </c>
       <c r="B59" s="0" t="inlineStr">
         <is>
-          <t>2833</t>
+          <t>9067</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="0" t="inlineStr">
         <is>
-          <t>greeting_nod.csv</t>
+          <t>dst-foot-play.csv</t>
         </is>
       </c>
       <c r="B60" s="0" t="inlineStr">
         <is>
-          <t>933</t>
+          <t>56067</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="0" t="inlineStr">
         <is>
-          <t>greeting_shake_hand.csv</t>
+          <t>FGT_lets_dance.csv</t>
         </is>
       </c>
       <c r="B61" s="0" t="inlineStr">
         <is>
-          <t>6900</t>
+          <t>142333</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="0" t="inlineStr">
         <is>
-          <t>greeting_wave_double.csv</t>
+          <t>greetings_wave.csv</t>
         </is>
       </c>
       <c r="B62" s="0" t="inlineStr">
         <is>
-          <t>6133</t>
+          <t>7500</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="0" t="inlineStr">
         <is>
-          <t>greeting_wave_left.csv</t>
+          <t>greeting_bow_deep.csv</t>
         </is>
       </c>
       <c r="B63" s="0" t="inlineStr">
         <is>
-          <t>6133</t>
+          <t>6400</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="0" t="inlineStr">
         <is>
-          <t>iso-f2h-catch-rockroll-seq.csv</t>
+          <t>greeting_bow_small.csv</t>
         </is>
       </c>
       <c r="B64" s="0" t="inlineStr">
         <is>
-          <t>29967</t>
+          <t>2833</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="0" t="inlineStr">
         <is>
-          <t>iso-forhead-balance.csv</t>
+          <t>greeting_nod.csv</t>
         </is>
       </c>
       <c r="B65" s="0" t="inlineStr">
         <is>
-          <t>8400</t>
+          <t>933</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="0" t="inlineStr">
         <is>
-          <t>iso-lowh2h-standonshoulder.csv</t>
+          <t>greeting_shake_hand.csv</t>
         </is>
       </c>
       <c r="B66" s="0" t="inlineStr">
         <is>
-          <t>43100</t>
+          <t>6900</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="0" t="inlineStr">
         <is>
-          <t>iso-shoulderbird-kneehandstand.csv</t>
+          <t>greeting_wave_double.csv</t>
         </is>
       </c>
       <c r="B67" s="0" t="inlineStr">
         <is>
-          <t>22167</t>
+          <t>6133</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="inlineStr">
         <is>
-          <t>pattern-3-limbs-referentie.csv</t>
+          <t>greeting_wave_left.csv</t>
         </is>
       </c>
       <c r="B68" s="0" t="inlineStr">
         <is>
-          <t>3333</t>
+          <t>6133</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="0" t="inlineStr">
         <is>
-          <t>pattern-3-limbs.csv</t>
+          <t>iso-f2h-catch-rockroll-seq.csv</t>
         </is>
       </c>
       <c r="B69" s="0" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>29967</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="0" t="inlineStr">
         <is>
-          <t>pattern-3-limbs2.csv</t>
+          <t>iso-forhead-balance.csv</t>
         </is>
       </c>
       <c r="B70" s="0" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>8400</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="0" t="inlineStr">
         <is>
-          <t>pose_180.csv</t>
+          <t>iso-lowh2h-standonshoulder.csv</t>
         </is>
       </c>
       <c r="B71" s="0" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>43100</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="inlineStr">
         <is>
-          <t>pose_handstand.csv</t>
+          <t>iso-shoulderbird-kneehandstand.csv</t>
         </is>
       </c>
       <c r="B72" s="0" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>22167</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="0" t="inlineStr">
         <is>
-          <t>pose_handstand_oversplit.csv</t>
+          <t>pattern-3-limbs-referentie.csv</t>
         </is>
       </c>
       <c r="B73" s="0" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>3333</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="0" t="inlineStr">
         <is>
-          <t>pose_handstand_split.csv</t>
+          <t>pattern-3-limbs.csv</t>
         </is>
       </c>
       <c r="B74" s="0" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>2000</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="inlineStr">
         <is>
-          <t>pose_planche.csv</t>
+          <t>pattern-3-limbs2.csv</t>
         </is>
       </c>
       <c r="B75" s="0" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="inlineStr">
         <is>
-          <t>pose_scorpion.csv</t>
+          <t>pose_180.csv</t>
         </is>
       </c>
       <c r="B76" s="0" t="inlineStr">
@@ -2389,7 +2389,7 @@
     <row r="77">
       <c r="A77" s="0" t="inlineStr">
         <is>
-          <t>pose_seven.csv</t>
+          <t>pose_handstand.csv</t>
         </is>
       </c>
       <c r="B77" s="0" t="inlineStr">
@@ -2401,7 +2401,7 @@
     <row r="78">
       <c r="A78" s="0" t="inlineStr">
         <is>
-          <t>pose_sit.csv</t>
+          <t>pose_handstand_oversplit.csv</t>
         </is>
       </c>
       <c r="B78" s="0" t="inlineStr">
@@ -2413,7 +2413,7 @@
     <row r="79">
       <c r="A79" s="0" t="inlineStr">
         <is>
-          <t>pose_split_l.csv</t>
+          <t>pose_handstand_split.csv</t>
         </is>
       </c>
       <c r="B79" s="0" t="inlineStr">
@@ -2425,7 +2425,7 @@
     <row r="80">
       <c r="A80" s="0" t="inlineStr">
         <is>
-          <t>pose_stand.csv</t>
+          <t>pose_planche.csv</t>
         </is>
       </c>
       <c r="B80" s="0" t="inlineStr">
@@ -2437,7 +2437,7 @@
     <row r="81">
       <c r="A81" s="0" t="inlineStr">
         <is>
-          <t>pose_stand_legs_only.csv</t>
+          <t>pose_scorpion.csv</t>
         </is>
       </c>
       <c r="B81" s="0" t="inlineStr">
@@ -2449,7 +2449,7 @@
     <row r="82">
       <c r="A82" s="0" t="inlineStr">
         <is>
-          <t>pose_table.csv</t>
+          <t>pose_seven.csv</t>
         </is>
       </c>
       <c r="B82" s="0" t="inlineStr">
@@ -2461,7 +2461,7 @@
     <row r="83">
       <c r="A83" s="0" t="inlineStr">
         <is>
-          <t>pose_yoga_dog.csv</t>
+          <t>pose_sit.csv</t>
         </is>
       </c>
       <c r="B83" s="0" t="inlineStr">
@@ -2473,103 +2473,103 @@
     <row r="84">
       <c r="A84" s="0" t="inlineStr">
         <is>
-          <t>quick_01-backup.csv</t>
+          <t>pose_split_l.csv</t>
         </is>
       </c>
       <c r="B84" s="0" t="inlineStr">
         <is>
-          <t>102833</t>
+          <t>33</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="0" t="inlineStr">
         <is>
-          <t>repeat_hump_arms_legs_samedir_16s.csv</t>
+          <t>pose_stand.csv</t>
         </is>
       </c>
       <c r="B85" s="0" t="inlineStr">
         <is>
-          <t>16000</t>
+          <t>33</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="inlineStr">
         <is>
-          <t>repeat_hump_large_4s.csv</t>
+          <t>pose_stand_legs_only.csv</t>
         </is>
       </c>
       <c r="B86" s="0" t="inlineStr">
         <is>
-          <t>4000</t>
+          <t>33</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="0" t="inlineStr">
         <is>
-          <t>repeat_hump_medium_3s.csv</t>
+          <t>pose_table.csv</t>
         </is>
       </c>
       <c r="B87" s="0" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>33</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="0" t="inlineStr">
         <is>
-          <t>repeat_hump_medium_arms_3s.csv</t>
+          <t>pose_yoga_dog.csv</t>
         </is>
       </c>
       <c r="B88" s="0" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>33</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="0" t="inlineStr">
         <is>
-          <t>repeat_hump_medium_arms_linear_3s.csv</t>
+          <t>quick_01-backup.csv</t>
         </is>
       </c>
       <c r="B89" s="0" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>102833</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="0" t="inlineStr">
         <is>
-          <t>repeat_hump_medium_windup_5s.csv</t>
+          <t>repeat_hump_arms_legs_samedir_16s.csv</t>
         </is>
       </c>
       <c r="B90" s="0" t="inlineStr">
         <is>
-          <t>5000</t>
+          <t>16000</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="0" t="inlineStr">
         <is>
-          <t>repeat_hump_small_1s.csv</t>
+          <t>repeat_hump_large_4s.csv</t>
         </is>
       </c>
       <c r="B91" s="0" t="inlineStr">
         <is>
-          <t>1000</t>
+          <t>4000</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="0" t="inlineStr">
         <is>
-          <t>repeat_hump_small_3s.csv</t>
+          <t>repeat_hump_medium_3s.csv</t>
         </is>
       </c>
       <c r="B92" s="0" t="inlineStr">
@@ -2581,538 +2581,598 @@
     <row r="93">
       <c r="A93" s="0" t="inlineStr">
         <is>
-          <t>repeat_hump_XL_4s.csv</t>
+          <t>repeat_hump_medium_arms_3s.csv</t>
         </is>
       </c>
       <c r="B93" s="0" t="inlineStr">
         <is>
-          <t>4000</t>
+          <t>3000</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="inlineStr">
         <is>
-          <t>repeat_random_individual_10s.csv</t>
+          <t>repeat_hump_medium_arms_linear_3s.csv</t>
         </is>
       </c>
       <c r="B94" s="0" t="inlineStr">
         <is>
-          <t>10000</t>
+          <t>3000</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="0" t="inlineStr">
         <is>
-          <t>repeat_random_individual_20s.csv</t>
+          <t>repeat_hump_medium_windup_5s.csv</t>
         </is>
       </c>
       <c r="B95" s="0" t="inlineStr">
         <is>
-          <t>20000</t>
+          <t>5000</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="0" t="inlineStr">
         <is>
-          <t>repeat_random_individual_ease_20s.csv</t>
+          <t>repeat_hump_small_1s.csv</t>
         </is>
       </c>
       <c r="B96" s="0" t="inlineStr">
         <is>
-          <t>20000</t>
+          <t>1000</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="0" t="inlineStr">
         <is>
-          <t>repeat_random_individual_lin_20.csv</t>
+          <t>repeat_hump_small_3s.csv</t>
         </is>
       </c>
       <c r="B97" s="0" t="inlineStr">
         <is>
-          <t>20000</t>
+          <t>3000</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="0" t="inlineStr">
         <is>
-          <t>repeat_rotate_arms_16s.csv</t>
+          <t>repeat_hump_XL_4s.csv</t>
         </is>
       </c>
       <c r="B98" s="0" t="inlineStr">
         <is>
-          <t>16000</t>
+          <t>4000</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="0" t="inlineStr">
         <is>
-          <t>repeat_rotate_arms_legs_opp_16s.csv</t>
+          <t>repeat_random_individual_10s.csv</t>
         </is>
       </c>
       <c r="B99" s="0" t="inlineStr">
         <is>
-          <t>16000</t>
+          <t>10000</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="0" t="inlineStr">
         <is>
-          <t>repeat_rotate_arms_legs_samedir_16s.csv</t>
+          <t>repeat_random_individual_20s.csv</t>
         </is>
       </c>
       <c r="B100" s="0" t="inlineStr">
         <is>
-          <t>16000</t>
+          <t>20000</t>
         </is>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="0" t="inlineStr">
         <is>
-          <t>salto_d2_dans_acro_01.csv</t>
+          <t>repeat_random_individual_ease_20s.csv</t>
         </is>
       </c>
       <c r="B101" s="0" t="inlineStr">
         <is>
-          <t>60133</t>
+          <t>20000</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="0" t="inlineStr">
         <is>
-          <t>salto_d2_dans_acro_02.csv</t>
+          <t>repeat_random_individual_lin_20.csv</t>
         </is>
       </c>
       <c r="B102" s="0" t="inlineStr">
         <is>
-          <t>127033</t>
+          <t>20000</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="0" t="inlineStr">
         <is>
-          <t>shoulderbird-knee-tweakers.csv</t>
+          <t>repeat_rotate_arms_16s.csv</t>
         </is>
       </c>
       <c r="B103" s="0" t="inlineStr">
         <is>
-          <t>27967</t>
+          <t>16000</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="0" t="inlineStr">
         <is>
-          <t>tango-downward-dog-sequence.csv</t>
+          <t>repeat_rotate_arms_legs_opp_16s.csv</t>
         </is>
       </c>
       <c r="B104" s="0" t="inlineStr">
         <is>
-          <t>32000</t>
+          <t>16000</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="0" t="inlineStr">
         <is>
-          <t>tango-sequence-dst-alternate-end.csv</t>
+          <t>repeat_rotate_arms_legs_samedir_16s.csv</t>
         </is>
       </c>
       <c r="B105" s="0" t="inlineStr">
         <is>
-          <t>110900</t>
+          <t>16000</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="0" t="inlineStr">
         <is>
-          <t>tango-sequence-dst-splits.csv</t>
+          <t>salto_d2_dans_acro_01.csv</t>
         </is>
       </c>
       <c r="B106" s="0" t="inlineStr">
         <is>
-          <t>6500</t>
+          <t>60133</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="0" t="inlineStr">
         <is>
-          <t>tango-sequence-dst-splits2.csv</t>
+          <t>salto_d2_dans_acro_02.csv</t>
         </is>
       </c>
       <c r="B107" s="0" t="inlineStr">
         <is>
-          <t>13500</t>
+          <t>127033</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="0" t="inlineStr">
         <is>
-          <t>tango-sequence-dst-stoeltje.csv</t>
+          <t>shoulderbird-knee-tweakers.csv</t>
         </is>
       </c>
       <c r="B108" s="0" t="inlineStr">
         <is>
-          <t>8567</t>
+          <t>27967</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="0" t="inlineStr">
         <is>
-          <t>tango-sequence-dst.csv</t>
+          <t>tango-downward-dog-sequence.csv</t>
         </is>
       </c>
       <c r="B109" s="0" t="inlineStr">
         <is>
-          <t>112233</t>
+          <t>32000</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="0" t="inlineStr">
         <is>
-          <t>test_3limbs.csv</t>
+          <t>tango-sequence-dst-alternate-end.csv</t>
         </is>
       </c>
       <c r="B110" s="0" t="inlineStr">
         <is>
-          <t>4000</t>
+          <t>110900</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="0" t="inlineStr">
         <is>
-          <t>test_cannonball.csv</t>
+          <t>tango-sequence-dst-splits.csv</t>
         </is>
       </c>
       <c r="B111" s="0" t="inlineStr">
         <is>
-          <t>24367</t>
+          <t>6500</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="inlineStr">
         <is>
-          <t>test_contra_finale.csv</t>
+          <t>tango-sequence-dst-splits2.csv</t>
         </is>
       </c>
       <c r="B112" s="0" t="inlineStr">
         <is>
-          <t>40833</t>
+          <t>13500</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="0" t="inlineStr">
         <is>
-          <t>test_dog.csv</t>
+          <t>tango-sequence-dst-stoeltje.csv</t>
         </is>
       </c>
       <c r="B113" s="0" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>8567</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="0" t="inlineStr">
         <is>
-          <t>test_flikflak_daniel.csv</t>
+          <t>tango-sequence-dst.csv</t>
         </is>
       </c>
       <c r="B114" s="0" t="inlineStr">
         <is>
-          <t>22633</t>
+          <t>112233</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="0" t="inlineStr">
         <is>
-          <t>test_flop_roll.csv</t>
+          <t>test_3limbs.csv</t>
         </is>
       </c>
       <c r="B115" s="0" t="inlineStr">
         <is>
-          <t>10100</t>
+          <t>4000</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="0" t="inlineStr">
         <is>
-          <t>test_fullrev.csv</t>
+          <t>test_cannonball.csv</t>
         </is>
       </c>
       <c r="B116" s="0" t="inlineStr">
         <is>
-          <t>8000</t>
+          <t>24367</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="0" t="inlineStr">
         <is>
-          <t>test_multi_rev.csv</t>
+          <t>test_contra_finale.csv</t>
         </is>
       </c>
       <c r="B117" s="0" t="inlineStr">
         <is>
-          <t>20000</t>
+          <t>40833</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="0" t="inlineStr">
         <is>
-          <t>test_rockroll.csv</t>
+          <t>test_dog.csv</t>
         </is>
       </c>
       <c r="B118" s="0" t="inlineStr">
         <is>
-          <t>32967</t>
+          <t>2000</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="0" t="inlineStr">
         <is>
-          <t>travel_walk_96bmp.csv</t>
+          <t>test_flikflak_daniel.csv</t>
         </is>
       </c>
       <c r="B119" s="0" t="inlineStr">
         <is>
-          <t>1333</t>
+          <t>22633</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="0" t="inlineStr">
         <is>
-          <t>trick-backflip-pose.csv</t>
+          <t>test_flop_roll.csv</t>
         </is>
       </c>
       <c r="B120" s="0" t="inlineStr">
         <is>
-          <t>3000</t>
+          <t>10100</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="0" t="inlineStr">
         <is>
-          <t>trick-backflip1.csv</t>
+          <t>test_fullrev.csv</t>
         </is>
       </c>
       <c r="B121" s="0" t="inlineStr">
         <is>
-          <t>7933</t>
+          <t>8000</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="0" t="inlineStr">
         <is>
-          <t>trick-backflip2.csv</t>
+          <t>test_multi_rev.csv</t>
         </is>
       </c>
       <c r="B122" s="0" t="inlineStr">
         <is>
-          <t>12033</t>
+          <t>20000</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="0" t="inlineStr">
         <is>
-          <t>trick-backflip3.csv</t>
+          <t>test_rockroll.csv</t>
         </is>
       </c>
       <c r="B123" s="0" t="inlineStr">
         <is>
-          <t>13033</t>
+          <t>32967</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="0" t="inlineStr">
         <is>
-          <t>trick-backflip4.csv</t>
+          <t>travel_walk_96bmp.csv</t>
         </is>
       </c>
       <c r="B124" s="0" t="inlineStr">
         <is>
-          <t>13033</t>
+          <t>1333</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="0" t="inlineStr">
         <is>
-          <t>trick-ropeskipping.csv</t>
+          <t>trick-backflip-pose.csv</t>
         </is>
       </c>
       <c r="B125" s="0" t="inlineStr">
         <is>
-          <t>7000</t>
+          <t>3000</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="0" t="inlineStr">
         <is>
-          <t>trick-ropeskipping2.csv</t>
+          <t>trick-backflip1.csv</t>
         </is>
       </c>
       <c r="B126" s="0" t="inlineStr">
         <is>
-          <t>3900</t>
+          <t>7933</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="0" t="inlineStr">
         <is>
-          <t>trick-walkover.csv</t>
+          <t>trick-backflip2.csv</t>
         </is>
       </c>
       <c r="B127" s="0" t="inlineStr">
         <is>
-          <t>21000</t>
+          <t>12033</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="0" t="inlineStr">
         <is>
-          <t>trick-walkover2.csv</t>
+          <t>trick-backflip3.csv</t>
         </is>
       </c>
       <c r="B128" s="0" t="inlineStr">
         <is>
-          <t>18000</t>
+          <t>13033</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="0" t="inlineStr">
         <is>
-          <t>walk_backwards.csv</t>
+          <t>trick-backflip4.csv</t>
         </is>
       </c>
       <c r="B129" s="0" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>13033</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="0" t="inlineStr">
         <is>
-          <t>walk_forwards.csv</t>
+          <t>trick-ropeskipping.csv</t>
         </is>
       </c>
       <c r="B130" s="0" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>7000</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="0" t="inlineStr">
         <is>
-          <t>walk_large.csv</t>
+          <t>trick-ropeskipping2.csv</t>
         </is>
       </c>
       <c r="B131" s="0" t="inlineStr">
         <is>
-          <t>2000</t>
+          <t>3900</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="0" t="inlineStr">
         <is>
-          <t>walk_normal.csv</t>
+          <t>trick-walkover.csv</t>
         </is>
       </c>
       <c r="B132" s="0" t="inlineStr">
         <is>
-          <t>1600</t>
+          <t>21000</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="0" t="inlineStr">
         <is>
+          <t>trick-walkover2.csv</t>
+        </is>
+      </c>
+      <c r="B133" s="0" t="inlineStr">
+        <is>
+          <t>18000</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="0" t="inlineStr">
+        <is>
+          <t>walk_backwards.csv</t>
+        </is>
+      </c>
+      <c r="B134" s="0" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="0" t="inlineStr">
+        <is>
+          <t>walk_forwards.csv</t>
+        </is>
+      </c>
+      <c r="B135" s="0" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="0" t="inlineStr">
+        <is>
+          <t>walk_large.csv</t>
+        </is>
+      </c>
+      <c r="B136" s="0" t="inlineStr">
+        <is>
+          <t>2000</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="0" t="inlineStr">
+        <is>
+          <t>walk_normal.csv</t>
+        </is>
+      </c>
+      <c r="B137" s="0" t="inlineStr">
+        <is>
+          <t>1600</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="0" t="inlineStr">
+        <is>
           <t>walk_zombie.csv</t>
         </is>
       </c>
-      <c r="B133" s="0" t="inlineStr">
+      <c r="B138" s="0" t="inlineStr">
         <is>
           <t>1600</t>
         </is>
       </c>
     </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
+    <row r="139">
+      <c r="A139" s="0" t="inlineStr">
         <is>
           <t>warmup_arm_swing.csv</t>
         </is>
       </c>
-      <c r="B134" t="inlineStr">
+      <c r="B139" s="0" t="inlineStr">
         <is>
           <t>23867</t>
         </is>
       </c>
     </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
+    <row r="140">
+      <c r="A140" s="0" t="inlineStr">
         <is>
           <t>warmup_leg_stretch.csv</t>
         </is>
       </c>
-      <c r="B135" t="inlineStr">
+      <c r="B140" s="0" t="inlineStr">
         <is>
           <t>19467</t>
         </is>
       </c>
     </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
+    <row r="141">
+      <c r="A141" s="0" t="inlineStr">
         <is>
           <t>warmup_shoulder_stretch.csv</t>
         </is>
       </c>
-      <c r="B136" t="inlineStr">
+      <c r="B141" s="0" t="inlineStr">
         <is>
           <t>15267</t>
         </is>
       </c>
     </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
+    <row r="142">
+      <c r="A142" s="0" t="inlineStr">
         <is>
           <t>warmup_situp.csv</t>
         </is>
       </c>
-      <c r="B137" t="inlineStr">
+      <c r="B142" s="0" t="inlineStr">
         <is>
           <t>5900</t>
         </is>

</xml_diff>